<commit_message>
my da add va test xong
</commit_message>
<xml_diff>
--- a/file/datasv.xlsx
+++ b/file/datasv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioCode\data_baitaplon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D879FA-6E20-459C-ADE8-E25644FF7FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AE0EC8-E906-4B0A-923A-9D7B5EA08E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,13 +418,13 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
sua lai tim va them
</commit_message>
<xml_diff>
--- a/file/datasv.xlsx
+++ b/file/datasv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioCode\data_baitaplon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AE0EC8-E906-4B0A-923A-9D7B5EA08E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D0ABA5-7506-42B5-9EFD-7466FBAFC912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>0017</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Khóa học</t>
+  </si>
+  <si>
+    <t>2019-2023</t>
   </si>
 </sst>
 </file>
@@ -415,19 +421,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -446,8 +453,11 @@
       <c r="F1" t="s">
         <v>21</v>
       </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,8 +476,11 @@
       <c r="F2" s="1">
         <v>909526211</v>
       </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -486,8 +499,11 @@
       <c r="F3" s="1">
         <v>909526211</v>
       </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -506,8 +522,11 @@
       <c r="F4" s="1">
         <v>909526211</v>
       </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -525,6 +544,9 @@
       </c>
       <c r="F5" s="1">
         <v>909526211</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
da sua xong giao dien cap nhat sinh vien
</commit_message>
<xml_diff>
--- a/file/datasv.xlsx
+++ b/file/datasv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioCode\data_baitaplon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D0ABA5-7506-42B5-9EFD-7466FBAFC912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDFE243-D3C0-472F-82EE-463E33D16FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G6" sqref="A6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,6 +549,11 @@
         <v>23</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sua loi thong bao
</commit_message>
<xml_diff>
--- a/file/datasv.xlsx
+++ b/file/datasv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAPTOP\Desktop\HK1-Nam4\Cong nghe moi\Do an\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioCode\data_baitaplon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FE1C63-4B57-4896-BADA-0C42BED33E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1913CC-D309-4DFC-8C33-2EE8CB732D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>đồng nai</t>
   </si>
@@ -84,19 +84,76 @@
     <t>Khóa học</t>
   </si>
   <si>
-    <t>2019-2023</t>
-  </si>
-  <si>
-    <t>0021</t>
-  </si>
-  <si>
-    <t>0022</t>
-  </si>
-  <si>
-    <t>0023</t>
-  </si>
-  <si>
-    <t>0024</t>
+    <t>0027</t>
+  </si>
+  <si>
+    <t>0028</t>
+  </si>
+  <si>
+    <t>0029</t>
+  </si>
+  <si>
+    <t>0030</t>
+  </si>
+  <si>
+    <t>0031</t>
+  </si>
+  <si>
+    <t>0032</t>
+  </si>
+  <si>
+    <t>0033</t>
+  </si>
+  <si>
+    <t>0034</t>
+  </si>
+  <si>
+    <t>0035</t>
+  </si>
+  <si>
+    <t>Văn E</t>
+  </si>
+  <si>
+    <t>Văn F</t>
+  </si>
+  <si>
+    <t>Văn G</t>
+  </si>
+  <si>
+    <t>Văn H</t>
+  </si>
+  <si>
+    <t>Văn Q</t>
+  </si>
+  <si>
+    <t>2000-11-7</t>
+  </si>
+  <si>
+    <t>2000-11-8</t>
+  </si>
+  <si>
+    <t>2000-11-9</t>
+  </si>
+  <si>
+    <t>2000-11-10</t>
+  </si>
+  <si>
+    <t>2000-11-11</t>
+  </si>
+  <si>
+    <t>909526212</t>
+  </si>
+  <si>
+    <t>909526213</t>
+  </si>
+  <si>
+    <t>909526214</t>
+  </si>
+  <si>
+    <t>909526215</t>
+  </si>
+  <si>
+    <t>2018-2022</t>
   </si>
 </sst>
 </file>
@@ -421,15 +478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
@@ -459,7 +516,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -477,12 +534,12 @@
         <v>909526211</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -496,16 +553,16 @@
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1">
-        <v>909526211</v>
+      <c r="F3" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -520,15 +577,15 @@
         <v>10</v>
       </c>
       <c r="F4" s="1">
-        <v>909526211</v>
+        <v>909526212</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -542,17 +599,127 @@
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="1">
-        <v>909526211</v>
+      <c r="F5" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1">
+        <v>909526213</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1">
+        <v>909526214</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="1">
+        <v>909526215</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>